<commit_message>
upgrade for add dd(Deleted) field
</commit_message>
<xml_diff>
--- a/org.shaneking.leon.persistence/src/test/java/sktest/leon/persistence/biz/tstFiles/WebPersistenceEntityBizTest_template_null_o.xlsx
+++ b/org.shaneking.leon.persistence/src/test/java/sktest/leon/persistence/biz/tstFiles/WebPersistenceEntityBizTest_template_null_o.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
   <si>
     <t/>
   </si>
@@ -20,6 +20,9 @@
     <t>id</t>
   </si>
   <si>
+    <t>dd</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
@@ -48,6 +51,9 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -140,10 +146,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
@@ -154,7 +160,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -162,15 +168,16 @@
   <cols>
     <col min="1" max="1" width="6.0" customWidth="true"/>
     <col min="2" max="2" width="6.0" customWidth="true"/>
-    <col min="3" max="3" width="14.0" customWidth="true"/>
-    <col min="4" max="4" width="32.0" customWidth="true"/>
-    <col min="5" max="5" width="30.0" customWidth="true"/>
-    <col min="6" max="6" width="14.0" customWidth="true"/>
-    <col min="7" max="7" width="16.0" customWidth="true"/>
-    <col min="8" max="8" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="6.0" customWidth="true"/>
+    <col min="4" max="4" width="14.0" customWidth="true"/>
+    <col min="5" max="5" width="32.0" customWidth="true"/>
+    <col min="6" max="6" width="30.0" customWidth="true"/>
+    <col min="7" max="7" width="14.0" customWidth="true"/>
+    <col min="8" max="8" width="16.0" customWidth="true"/>
     <col min="9" max="9" width="8.0" customWidth="true"/>
-    <col min="10" max="10" width="12.0" customWidth="true"/>
-    <col min="11" max="11" width="10.0" customWidth="true"/>
+    <col min="10" max="10" width="8.0" customWidth="true"/>
+    <col min="11" max="11" width="12.0" customWidth="true"/>
+    <col min="12" max="12" width="10.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.0" customHeight="true">
@@ -183,13 +190,13 @@
       <c r="C1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" t="s" s="2">
         <v>6</v>
       </c>
       <c r="G1" t="s" s="2">
@@ -198,28 +205,34 @@
       <c r="H1" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="J1" t="s" s="3">
+      <c r="J1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="K1" t="s" s="3">
+      <c r="K1" t="s" s="2">
         <v>11</v>
+      </c>
+      <c r="L1" t="s" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="2" ht="20.0" customHeight="true">
       <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="B2" t="s" s="4">
+        <v>13</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>